<commit_message>
minor notes and words
</commit_message>
<xml_diff>
--- a/phrx_words.xlsx
+++ b/phrx_words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felipe\Pictures\Phyrexian\phyrexian_search_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3391A950-8D37-44B3-84CF-F92D8A2E5101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5A441E-A7F4-4C7A-8527-90FEF9F50E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="578">
   <si>
     <t>Ability</t>
   </si>
@@ -1758,6 +1758,15 @@
   </si>
   <si>
     <t>ZvOTdLTd</t>
+  </si>
+  <si>
+    <t>LMvODdNx</t>
+  </si>
+  <si>
+    <t>TdQ-ZNvZwHZyMxZy_dE-ZGZx</t>
+  </si>
+  <si>
+    <t>TdLZy_d-ZHZvLDdNwGNy</t>
   </si>
 </sst>
 </file>
@@ -2599,10 +2608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C345"/>
+  <dimension ref="A1:C348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A331" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I348" sqref="I348"/>
+    <sheetView tabSelected="1" topLeftCell="A327" zoomScale="81" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C327" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4380,13 +4389,13 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>84</v>
+        <v>216</v>
       </c>
       <c r="B162" t="s">
-        <v>546</v>
+        <v>307</v>
       </c>
       <c r="C162" t="s">
-        <v>85</v>
+        <v>577</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -4394,43 +4403,43 @@
         <v>84</v>
       </c>
       <c r="B163" t="s">
-        <v>320</v>
+        <v>546</v>
       </c>
       <c r="C163" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B164" t="s">
         <v>320</v>
       </c>
       <c r="C164" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B165" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="C165" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>258</v>
+        <v>89</v>
       </c>
       <c r="B166" t="s">
-        <v>426</v>
+        <v>310</v>
       </c>
       <c r="C166" t="s">
-        <v>259</v>
+        <v>90</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -4438,65 +4447,65 @@
         <v>258</v>
       </c>
       <c r="B167" t="s">
-        <v>483</v>
+        <v>426</v>
       </c>
       <c r="C167" t="s">
-        <v>488</v>
+        <v>259</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>387</v>
+        <v>258</v>
       </c>
       <c r="B168" t="s">
-        <v>383</v>
-      </c>
-      <c r="C168" s="1" t="s">
-        <v>388</v>
+        <v>483</v>
+      </c>
+      <c r="C168" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>91</v>
+        <v>387</v>
       </c>
       <c r="B169" t="s">
-        <v>308</v>
-      </c>
-      <c r="C169" t="s">
-        <v>92</v>
+        <v>383</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B170" t="s">
-        <v>341</v>
+        <v>308</v>
       </c>
       <c r="C170" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>370</v>
+        <v>93</v>
       </c>
       <c r="B171" t="s">
-        <v>422</v>
+        <v>341</v>
       </c>
       <c r="C171" t="s">
-        <v>371</v>
+        <v>94</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>413</v>
+        <v>370</v>
       </c>
       <c r="B172" t="s">
-        <v>415</v>
-      </c>
-      <c r="C172" s="1" t="s">
-        <v>416</v>
+        <v>422</v>
+      </c>
+      <c r="C172" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -4506,52 +4515,52 @@
       <c r="B173" t="s">
         <v>415</v>
       </c>
-      <c r="C173" t="s">
-        <v>418</v>
+      <c r="C173" s="1" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>267</v>
+        <v>413</v>
       </c>
       <c r="B174" t="s">
-        <v>327</v>
+        <v>415</v>
       </c>
       <c r="C174" t="s">
-        <v>270</v>
+        <v>418</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>492</v>
+        <v>267</v>
       </c>
       <c r="B175" t="s">
-        <v>483</v>
+        <v>327</v>
       </c>
       <c r="C175" t="s">
-        <v>493</v>
+        <v>270</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>285</v>
+        <v>492</v>
       </c>
       <c r="B176" t="s">
-        <v>340</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>282</v>
+        <v>483</v>
+      </c>
+      <c r="C176" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>95</v>
+        <v>285</v>
       </c>
       <c r="B177" t="s">
-        <v>333</v>
-      </c>
-      <c r="C177" t="s">
-        <v>99</v>
+        <v>340</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
@@ -4559,10 +4568,10 @@
         <v>95</v>
       </c>
       <c r="B178" t="s">
-        <v>417</v>
+        <v>333</v>
       </c>
       <c r="C178" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
@@ -4570,21 +4579,21 @@
         <v>95</v>
       </c>
       <c r="B179" t="s">
-        <v>308</v>
+        <v>417</v>
       </c>
       <c r="C179" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B180" t="s">
-        <v>560</v>
+        <v>308</v>
       </c>
       <c r="C180" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -4592,10 +4601,10 @@
         <v>100</v>
       </c>
       <c r="B181" t="s">
-        <v>313</v>
+        <v>560</v>
       </c>
       <c r="C181" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
@@ -4603,10 +4612,10 @@
         <v>100</v>
       </c>
       <c r="B182" t="s">
-        <v>467</v>
+        <v>313</v>
       </c>
       <c r="C182" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
@@ -4614,32 +4623,32 @@
         <v>100</v>
       </c>
       <c r="B183" t="s">
-        <v>500</v>
-      </c>
-      <c r="C183" s="1" t="s">
-        <v>516</v>
+        <v>467</v>
+      </c>
+      <c r="C183" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>538</v>
+        <v>100</v>
       </c>
       <c r="B184" t="s">
-        <v>525</v>
-      </c>
-      <c r="C184" t="s">
-        <v>539</v>
+        <v>500</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>102</v>
+        <v>538</v>
       </c>
       <c r="B185" t="s">
-        <v>320</v>
+        <v>525</v>
       </c>
       <c r="C185" t="s">
-        <v>105</v>
+        <v>539</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -4647,10 +4656,10 @@
         <v>102</v>
       </c>
       <c r="B186" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C186" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
@@ -4658,10 +4667,10 @@
         <v>102</v>
       </c>
       <c r="B187" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C187" t="s">
-        <v>207</v>
+        <v>104</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
@@ -4669,54 +4678,54 @@
         <v>102</v>
       </c>
       <c r="B188" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="C188" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>372</v>
+        <v>102</v>
       </c>
       <c r="B189" t="s">
-        <v>430</v>
+        <v>329</v>
       </c>
       <c r="C189" t="s">
-        <v>373</v>
+        <v>103</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>406</v>
+        <v>372</v>
       </c>
       <c r="B190" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C190" t="s">
-        <v>407</v>
+        <v>373</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="B191" t="s">
-        <v>399</v>
+        <v>429</v>
       </c>
       <c r="C191" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>489</v>
+        <v>401</v>
       </c>
       <c r="B192" t="s">
-        <v>483</v>
-      </c>
-      <c r="C192" s="1" t="s">
-        <v>490</v>
+        <v>399</v>
+      </c>
+      <c r="C192" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
@@ -4724,21 +4733,21 @@
         <v>489</v>
       </c>
       <c r="B193" t="s">
-        <v>525</v>
-      </c>
-      <c r="C193" t="s">
-        <v>539</v>
+        <v>483</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>106</v>
+        <v>489</v>
       </c>
       <c r="B194" t="s">
-        <v>350</v>
+        <v>525</v>
       </c>
       <c r="C194" t="s">
-        <v>107</v>
+        <v>539</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
@@ -4746,10 +4755,10 @@
         <v>106</v>
       </c>
       <c r="B195" t="s">
-        <v>338</v>
+        <v>350</v>
       </c>
       <c r="C195" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -4757,32 +4766,32 @@
         <v>106</v>
       </c>
       <c r="B196" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C196" t="s">
-        <v>274</v>
+        <v>108</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B197" t="s">
-        <v>341</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>238</v>
+        <v>340</v>
+      </c>
+      <c r="C197" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B198" t="s">
-        <v>308</v>
-      </c>
-      <c r="C198" t="s">
-        <v>112</v>
+        <v>341</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
@@ -4790,10 +4799,10 @@
         <v>110</v>
       </c>
       <c r="B199" t="s">
-        <v>481</v>
+        <v>308</v>
       </c>
       <c r="C199" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
@@ -4801,10 +4810,10 @@
         <v>110</v>
       </c>
       <c r="B200" t="s">
-        <v>308</v>
+        <v>481</v>
       </c>
       <c r="C200" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -4815,7 +4824,7 @@
         <v>308</v>
       </c>
       <c r="C201" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
@@ -4823,21 +4832,21 @@
         <v>110</v>
       </c>
       <c r="B202" t="s">
-        <v>500</v>
+        <v>308</v>
       </c>
       <c r="C202" t="s">
-        <v>505</v>
+        <v>113</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>456</v>
+        <v>110</v>
       </c>
       <c r="B203" t="s">
-        <v>451</v>
+        <v>500</v>
       </c>
       <c r="C203" t="s">
-        <v>457</v>
+        <v>505</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.3">
@@ -4853,13 +4862,13 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>115</v>
+        <v>456</v>
       </c>
       <c r="B205" t="s">
-        <v>338</v>
+        <v>451</v>
       </c>
       <c r="C205" t="s">
-        <v>116</v>
+        <v>457</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
@@ -4867,32 +4876,32 @@
         <v>115</v>
       </c>
       <c r="B206" t="s">
-        <v>451</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>452</v>
+        <v>338</v>
+      </c>
+      <c r="C206" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>427</v>
+        <v>115</v>
       </c>
       <c r="B207" t="s">
-        <v>423</v>
+        <v>451</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>428</v>
+        <v>452</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>273</v>
+        <v>427</v>
       </c>
       <c r="B208" t="s">
-        <v>559</v>
-      </c>
-      <c r="C208" t="s">
-        <v>274</v>
+        <v>423</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
@@ -4900,32 +4909,32 @@
         <v>273</v>
       </c>
       <c r="B209" t="s">
-        <v>317</v>
+        <v>559</v>
       </c>
       <c r="C209" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B210" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C210" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>117</v>
+        <v>271</v>
       </c>
       <c r="B211" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="C211" t="s">
-        <v>120</v>
+        <v>272</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
@@ -4933,10 +4942,10 @@
         <v>117</v>
       </c>
       <c r="B212" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
       <c r="C212" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -4947,18 +4956,18 @@
         <v>338</v>
       </c>
       <c r="C213" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B214" t="s">
-        <v>314</v>
+        <v>338</v>
       </c>
       <c r="C214" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
@@ -4966,10 +4975,10 @@
         <v>121</v>
       </c>
       <c r="B215" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C215" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
@@ -4977,43 +4986,43 @@
         <v>121</v>
       </c>
       <c r="B216" t="s">
-        <v>451</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>453</v>
+        <v>320</v>
+      </c>
+      <c r="C216" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>414</v>
+        <v>121</v>
       </c>
       <c r="B217" t="s">
-        <v>415</v>
+        <v>451</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>416</v>
+        <v>453</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>123</v>
+        <v>414</v>
       </c>
       <c r="B218" t="s">
-        <v>313</v>
-      </c>
-      <c r="C218" t="s">
-        <v>124</v>
+        <v>415</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>515</v>
+        <v>123</v>
       </c>
       <c r="B219" t="s">
-        <v>500</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>516</v>
+        <v>313</v>
+      </c>
+      <c r="C219" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.3">
@@ -5021,109 +5030,109 @@
         <v>515</v>
       </c>
       <c r="B220" t="s">
-        <v>525</v>
-      </c>
-      <c r="C220" t="s">
-        <v>539</v>
+        <v>500</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>125</v>
+        <v>515</v>
       </c>
       <c r="B221" t="s">
-        <v>341</v>
-      </c>
-      <c r="C221" s="1" t="s">
-        <v>237</v>
+        <v>525</v>
+      </c>
+      <c r="C221" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>479</v>
+        <v>515</v>
       </c>
       <c r="B222" t="s">
-        <v>463</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>480</v>
+        <v>332</v>
+      </c>
+      <c r="C222" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B223" t="s">
-        <v>324</v>
-      </c>
-      <c r="C223" t="s">
-        <v>127</v>
+        <v>341</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>126</v>
+        <v>479</v>
       </c>
       <c r="B224" t="s">
-        <v>332</v>
-      </c>
-      <c r="C224" t="s">
-        <v>262</v>
+        <v>463</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B225" t="s">
-        <v>473</v>
+        <v>324</v>
       </c>
       <c r="C225" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B226" t="s">
-        <v>306</v>
+        <v>332</v>
       </c>
       <c r="C226" t="s">
-        <v>130</v>
+        <v>262</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>411</v>
+        <v>128</v>
       </c>
       <c r="B227" t="s">
-        <v>399</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>412</v>
+        <v>473</v>
+      </c>
+      <c r="C227" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>431</v>
+        <v>128</v>
       </c>
       <c r="B228" t="s">
-        <v>423</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>432</v>
+        <v>306</v>
+      </c>
+      <c r="C228" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
       <c r="B229" t="s">
-        <v>423</v>
-      </c>
-      <c r="C229" t="s">
-        <v>433</v>
+        <v>399</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.3">
@@ -5131,32 +5140,32 @@
         <v>431</v>
       </c>
       <c r="B230" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>131</v>
+        <v>431</v>
       </c>
       <c r="B231" t="s">
-        <v>341</v>
+        <v>423</v>
       </c>
       <c r="C231" t="s">
-        <v>134</v>
+        <v>433</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>131</v>
+        <v>431</v>
       </c>
       <c r="B232" t="s">
-        <v>343</v>
-      </c>
-      <c r="C232" t="s">
-        <v>133</v>
+        <v>440</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.3">
@@ -5164,10 +5173,10 @@
         <v>131</v>
       </c>
       <c r="B233" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="C233" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.3">
@@ -5175,43 +5184,43 @@
         <v>131</v>
       </c>
       <c r="B234" t="s">
-        <v>450</v>
+        <v>343</v>
       </c>
       <c r="C234" t="s">
-        <v>289</v>
+        <v>133</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>376</v>
+        <v>131</v>
       </c>
       <c r="B235" t="s">
-        <v>364</v>
+        <v>307</v>
       </c>
       <c r="C235" t="s">
-        <v>377</v>
+        <v>132</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B236" t="s">
-        <v>325</v>
+        <v>450</v>
       </c>
       <c r="C236" t="s">
-        <v>136</v>
+        <v>289</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>135</v>
+        <v>376</v>
       </c>
       <c r="B237" t="s">
-        <v>565</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>236</v>
+        <v>364</v>
+      </c>
+      <c r="C237" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
@@ -5219,10 +5228,10 @@
         <v>135</v>
       </c>
       <c r="B238" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="C238" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
@@ -5230,10 +5239,10 @@
         <v>135</v>
       </c>
       <c r="B239" t="s">
-        <v>563</v>
-      </c>
-      <c r="C239" t="s">
-        <v>566</v>
+        <v>565</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
@@ -5241,32 +5250,32 @@
         <v>135</v>
       </c>
       <c r="B240" t="s">
-        <v>563</v>
+        <v>313</v>
       </c>
       <c r="C240" t="s">
-        <v>567</v>
+        <v>137</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B241" t="s">
-        <v>351</v>
-      </c>
-      <c r="C241" s="1" t="s">
-        <v>235</v>
+        <v>563</v>
+      </c>
+      <c r="C241" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B242" t="s">
-        <v>341</v>
+        <v>563</v>
       </c>
       <c r="C242" t="s">
-        <v>139</v>
+        <v>567</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
@@ -5274,10 +5283,10 @@
         <v>138</v>
       </c>
       <c r="B243" t="s">
-        <v>338</v>
-      </c>
-      <c r="C243" t="s">
-        <v>118</v>
+        <v>351</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
@@ -5285,10 +5294,10 @@
         <v>138</v>
       </c>
       <c r="B244" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="C244" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
@@ -5296,10 +5305,10 @@
         <v>138</v>
       </c>
       <c r="B245" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C245" t="s">
-        <v>286</v>
+        <v>118</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
@@ -5307,43 +5316,43 @@
         <v>138</v>
       </c>
       <c r="B246" t="s">
-        <v>348</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>298</v>
+        <v>307</v>
+      </c>
+      <c r="C246" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>265</v>
+        <v>138</v>
       </c>
       <c r="B247" t="s">
-        <v>317</v>
-      </c>
-      <c r="C247" s="1" t="s">
-        <v>266</v>
+        <v>337</v>
+      </c>
+      <c r="C247" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>251</v>
+        <v>138</v>
       </c>
       <c r="B248" t="s">
-        <v>467</v>
-      </c>
-      <c r="C248" t="s">
-        <v>101</v>
+        <v>348</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="B249" t="s">
-        <v>442</v>
-      </c>
-      <c r="C249" t="s">
-        <v>252</v>
+        <v>317</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
@@ -5351,428 +5360,428 @@
         <v>251</v>
       </c>
       <c r="B250" t="s">
-        <v>500</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>516</v>
+        <v>467</v>
+      </c>
+      <c r="C250" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>140</v>
+        <v>251</v>
       </c>
       <c r="B251" t="s">
-        <v>320</v>
+        <v>442</v>
       </c>
       <c r="C251" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>140</v>
+        <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>330</v>
-      </c>
-      <c r="C252" t="s">
-        <v>18</v>
+        <v>500</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B253" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C253" t="s">
-        <v>454</v>
+        <v>19</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B254" t="s">
-        <v>530</v>
+        <v>330</v>
       </c>
       <c r="C254" t="s">
-        <v>455</v>
+        <v>18</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>520</v>
+        <v>141</v>
       </c>
       <c r="B255" t="s">
-        <v>500</v>
+        <v>325</v>
       </c>
       <c r="C255" t="s">
-        <v>521</v>
+        <v>454</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B256" t="s">
-        <v>562</v>
+        <v>530</v>
       </c>
       <c r="C256" t="s">
-        <v>143</v>
+        <v>455</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>144</v>
+        <v>520</v>
       </c>
       <c r="B257" t="s">
-        <v>307</v>
+        <v>500</v>
       </c>
       <c r="C257" t="s">
-        <v>145</v>
+        <v>521</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="B258" t="s">
-        <v>308</v>
+        <v>332</v>
       </c>
       <c r="C258" t="s">
-        <v>551</v>
+        <v>576</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B259" t="s">
-        <v>312</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>234</v>
+        <v>562</v>
+      </c>
+      <c r="C259" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>469</v>
+        <v>144</v>
       </c>
       <c r="B260" t="s">
-        <v>463</v>
+        <v>307</v>
       </c>
       <c r="C260" t="s">
-        <v>470</v>
+        <v>145</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>253</v>
+        <v>550</v>
       </c>
       <c r="B261" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
       <c r="C261" t="s">
-        <v>254</v>
+        <v>551</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B262" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>147</v>
+        <v>469</v>
       </c>
       <c r="B263" t="s">
-        <v>325</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>233</v>
+        <v>463</v>
+      </c>
+      <c r="C263" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>147</v>
+        <v>253</v>
       </c>
       <c r="B264" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C264" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B265" t="s">
-        <v>315</v>
-      </c>
-      <c r="C265" t="s">
-        <v>150</v>
+        <v>325</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B266" t="s">
-        <v>310</v>
-      </c>
-      <c r="C266" t="s">
-        <v>152</v>
+        <v>325</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>410</v>
+        <v>147</v>
       </c>
       <c r="B267" t="s">
-        <v>399</v>
+        <v>325</v>
       </c>
       <c r="C267" t="s">
-        <v>572</v>
+        <v>148</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B268" t="s">
-        <v>341</v>
+        <v>315</v>
       </c>
       <c r="C268" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B269" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C269" t="s">
-        <v>208</v>
+        <v>152</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="B270" t="s">
-        <v>383</v>
+        <v>399</v>
       </c>
       <c r="C270" t="s">
-        <v>390</v>
+        <v>572</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>502</v>
+        <v>153</v>
       </c>
       <c r="B271" t="s">
-        <v>500</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>503</v>
+        <v>341</v>
+      </c>
+      <c r="C271" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B272" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="C272" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>155</v>
+        <v>389</v>
       </c>
       <c r="B273" t="s">
-        <v>463</v>
+        <v>383</v>
       </c>
       <c r="C273" t="s">
-        <v>476</v>
+        <v>390</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>157</v>
+        <v>502</v>
       </c>
       <c r="B274" t="s">
-        <v>313</v>
-      </c>
-      <c r="C274" t="s">
-        <v>158</v>
+        <v>500</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>391</v>
+        <v>155</v>
       </c>
       <c r="B275" t="s">
-        <v>383</v>
+        <v>309</v>
       </c>
       <c r="C275" t="s">
-        <v>392</v>
+        <v>156</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B276" t="s">
-        <v>343</v>
+        <v>463</v>
       </c>
       <c r="C276" t="s">
-        <v>160</v>
+        <v>476</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B277" t="s">
-        <v>352</v>
+        <v>313</v>
       </c>
       <c r="C277" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>161</v>
+        <v>391</v>
       </c>
       <c r="B278" t="s">
-        <v>341</v>
+        <v>383</v>
       </c>
       <c r="C278" t="s">
-        <v>164</v>
+        <v>392</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B279" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="C279" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>424</v>
+        <v>161</v>
       </c>
       <c r="B280" t="s">
-        <v>423</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>425</v>
+        <v>352</v>
+      </c>
+      <c r="C280" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B281" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="C281" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>301</v>
+        <v>161</v>
       </c>
       <c r="B282" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="C282" t="s">
-        <v>302</v>
+        <v>162</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>167</v>
+        <v>424</v>
       </c>
       <c r="B283" t="s">
-        <v>313</v>
-      </c>
-      <c r="C283" t="s">
-        <v>168</v>
+        <v>423</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B284" t="s">
-        <v>423</v>
+        <v>331</v>
       </c>
       <c r="C284" t="s">
-        <v>436</v>
+        <v>166</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>508</v>
+        <v>301</v>
       </c>
       <c r="B285" t="s">
-        <v>500</v>
+        <v>353</v>
       </c>
       <c r="C285" t="s">
-        <v>509</v>
+        <v>302</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B286" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="C286" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B287" t="s">
-        <v>362</v>
+        <v>423</v>
       </c>
       <c r="C287" t="s">
-        <v>171</v>
+        <v>436</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>169</v>
+        <v>508</v>
       </c>
       <c r="B288" t="s">
-        <v>314</v>
+        <v>500</v>
       </c>
       <c r="C288" t="s">
-        <v>122</v>
+        <v>509</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.3">
@@ -5780,10 +5789,10 @@
         <v>169</v>
       </c>
       <c r="B289" t="s">
-        <v>307</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>230</v>
+        <v>321</v>
+      </c>
+      <c r="C289" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.3">
@@ -5791,230 +5800,230 @@
         <v>169</v>
       </c>
       <c r="B290" t="s">
-        <v>525</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>548</v>
+        <v>362</v>
+      </c>
+      <c r="C290" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>465</v>
+        <v>169</v>
       </c>
       <c r="B291" t="s">
-        <v>463</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>466</v>
+        <v>314</v>
+      </c>
+      <c r="C291" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>557</v>
+        <v>169</v>
       </c>
       <c r="B292" t="s">
-        <v>310</v>
-      </c>
-      <c r="C292" t="s">
-        <v>558</v>
+        <v>307</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>296</v>
+        <v>169</v>
       </c>
       <c r="B293" t="s">
-        <v>337</v>
-      </c>
-      <c r="C293" t="s">
-        <v>297</v>
+        <v>525</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>290</v>
+        <v>465</v>
       </c>
       <c r="B294" t="s">
-        <v>354</v>
-      </c>
-      <c r="C294" t="s">
-        <v>291</v>
+        <v>463</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>393</v>
+        <v>557</v>
       </c>
       <c r="B295" t="s">
-        <v>383</v>
+        <v>310</v>
       </c>
       <c r="C295" t="s">
-        <v>394</v>
+        <v>558</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>98</v>
+        <v>296</v>
       </c>
       <c r="B296" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="C296" t="s">
-        <v>172</v>
+        <v>297</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>173</v>
+        <v>290</v>
       </c>
       <c r="B297" t="s">
-        <v>309</v>
+        <v>354</v>
       </c>
       <c r="C297" t="s">
-        <v>174</v>
+        <v>291</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>175</v>
+        <v>393</v>
       </c>
       <c r="B298" t="s">
-        <v>313</v>
+        <v>383</v>
       </c>
       <c r="C298" t="s">
-        <v>176</v>
+        <v>394</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>175</v>
+        <v>98</v>
       </c>
       <c r="B299" t="s">
-        <v>308</v>
+        <v>355</v>
       </c>
       <c r="C299" t="s">
-        <v>112</v>
+        <v>172</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B300" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C300" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B301" t="s">
-        <v>528</v>
+        <v>313</v>
       </c>
       <c r="C301" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B302" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C302" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>361</v>
+        <v>175</v>
       </c>
       <c r="B303" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="C303" t="s">
-        <v>179</v>
+        <v>111</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="B304" t="s">
-        <v>316</v>
-      </c>
-      <c r="C304" s="1" t="s">
-        <v>229</v>
+        <v>528</v>
+      </c>
+      <c r="C304" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="B305" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C305" t="s">
-        <v>211</v>
+        <v>120</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>210</v>
+        <v>361</v>
       </c>
       <c r="B306" t="s">
-        <v>451</v>
-      </c>
-      <c r="C306" s="1" t="s">
-        <v>229</v>
+        <v>329</v>
+      </c>
+      <c r="C306" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>460</v>
+        <v>210</v>
       </c>
       <c r="B307" t="s">
-        <v>451</v>
-      </c>
-      <c r="C307" t="s">
-        <v>461</v>
+        <v>316</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="B308" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C308" t="s">
-        <v>6</v>
+        <v>211</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="B309" t="s">
-        <v>313</v>
-      </c>
-      <c r="C309" t="s">
-        <v>32</v>
+        <v>451</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>180</v>
+        <v>460</v>
       </c>
       <c r="B310" t="s">
-        <v>483</v>
+        <v>451</v>
       </c>
       <c r="C310" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.3">
@@ -6022,10 +6031,10 @@
         <v>180</v>
       </c>
       <c r="B311" t="s">
-        <v>500</v>
+        <v>313</v>
       </c>
       <c r="C311" t="s">
-        <v>511</v>
+        <v>6</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.3">
@@ -6033,120 +6042,120 @@
         <v>180</v>
       </c>
       <c r="B312" t="s">
-        <v>525</v>
+        <v>313</v>
       </c>
       <c r="C312" t="s">
-        <v>545</v>
+        <v>32</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>512</v>
+        <v>180</v>
       </c>
       <c r="B313" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
       <c r="C313" t="s">
-        <v>513</v>
+        <v>488</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B314" t="s">
-        <v>326</v>
+        <v>500</v>
       </c>
       <c r="C314" t="s">
-        <v>182</v>
+        <v>511</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B315" t="s">
-        <v>483</v>
+        <v>525</v>
       </c>
       <c r="C315" t="s">
-        <v>496</v>
+        <v>545</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>471</v>
+        <v>512</v>
       </c>
       <c r="B316" t="s">
-        <v>463</v>
-      </c>
-      <c r="C316" s="1" t="s">
-        <v>472</v>
+        <v>500</v>
+      </c>
+      <c r="C316" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B317" t="s">
-        <v>312</v>
+        <v>326</v>
       </c>
       <c r="C317" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B318" t="s">
-        <v>563</v>
-      </c>
-      <c r="C318" s="1" t="s">
-        <v>569</v>
+        <v>483</v>
+      </c>
+      <c r="C318" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>183</v>
+        <v>471</v>
       </c>
       <c r="B319" t="s">
-        <v>563</v>
+        <v>463</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>570</v>
+        <v>472</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B320" t="s">
-        <v>497</v>
+        <v>312</v>
       </c>
       <c r="C320" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B321" t="s">
-        <v>329</v>
-      </c>
-      <c r="C321" t="s">
-        <v>188</v>
+        <v>563</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B322" t="s">
-        <v>312</v>
-      </c>
-      <c r="C322" t="s">
-        <v>186</v>
+        <v>563</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.3">
@@ -6154,10 +6163,10 @@
         <v>185</v>
       </c>
       <c r="B323" t="s">
-        <v>320</v>
+        <v>497</v>
       </c>
       <c r="C323" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.3">
@@ -6165,246 +6174,279 @@
         <v>185</v>
       </c>
       <c r="B324" t="s">
-        <v>531</v>
-      </c>
-      <c r="C324" s="1" t="s">
-        <v>453</v>
+        <v>329</v>
+      </c>
+      <c r="C324" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="B325" t="s">
-        <v>316</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>227</v>
+        <v>312</v>
+      </c>
+      <c r="C325" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>474</v>
+        <v>185</v>
       </c>
       <c r="B326" t="s">
-        <v>463</v>
+        <v>320</v>
       </c>
       <c r="C326" t="s">
-        <v>475</v>
+        <v>189</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>474</v>
+        <v>185</v>
       </c>
       <c r="B327" t="s">
-        <v>308</v>
-      </c>
-      <c r="C327" t="s">
-        <v>113</v>
+        <v>531</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B328" t="s">
-        <v>312</v>
-      </c>
-      <c r="C328" t="s">
-        <v>225</v>
+        <v>316</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>524</v>
+        <v>474</v>
       </c>
       <c r="B329" t="s">
-        <v>525</v>
+        <v>463</v>
       </c>
       <c r="C329" t="s">
-        <v>526</v>
+        <v>475</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>190</v>
+        <v>474</v>
       </c>
       <c r="B330" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C330" t="s">
-        <v>191</v>
+        <v>113</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="B331" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C331" t="s">
-        <v>122</v>
+        <v>225</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>192</v>
+        <v>524</v>
       </c>
       <c r="B332" t="s">
-        <v>405</v>
+        <v>525</v>
       </c>
       <c r="C332" t="s">
-        <v>193</v>
+        <v>526</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B333" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
       <c r="C333" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B334" t="s">
-        <v>341</v>
+        <v>314</v>
       </c>
       <c r="C334" t="s">
-        <v>196</v>
+        <v>122</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>368</v>
+        <v>192</v>
       </c>
       <c r="B335" t="s">
-        <v>364</v>
+        <v>405</v>
       </c>
       <c r="C335" t="s">
-        <v>369</v>
+        <v>193</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="B336" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="C336" t="s">
-        <v>277</v>
+        <v>195</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>276</v>
+        <v>194</v>
       </c>
       <c r="B337" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C337" t="s">
-        <v>295</v>
+        <v>196</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>197</v>
+        <v>368</v>
       </c>
       <c r="B338" t="s">
-        <v>306</v>
+        <v>364</v>
       </c>
       <c r="C338" t="s">
-        <v>198</v>
+        <v>369</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>197</v>
+        <v>276</v>
       </c>
       <c r="B339" t="s">
-        <v>309</v>
+        <v>340</v>
       </c>
       <c r="C339" t="s">
-        <v>199</v>
+        <v>277</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>197</v>
+        <v>276</v>
       </c>
       <c r="B340" t="s">
-        <v>338</v>
-      </c>
-      <c r="C340" s="1" t="s">
-        <v>231</v>
+        <v>337</v>
+      </c>
+      <c r="C340" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B341" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="C341" t="s">
-        <v>83</v>
+        <v>198</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B342" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="C342" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B343" t="s">
-        <v>306</v>
-      </c>
-      <c r="C343" t="s">
-        <v>130</v>
+        <v>338</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B344" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C344" t="s">
-        <v>202</v>
+        <v>83</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
+        <v>200</v>
+      </c>
+      <c r="B345" t="s">
+        <v>341</v>
+      </c>
+      <c r="C345" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="346" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
         <v>201</v>
       </c>
-      <c r="B345" t="s">
+      <c r="B346" t="s">
+        <v>306</v>
+      </c>
+      <c r="C346" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="347" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>201</v>
+      </c>
+      <c r="B347" t="s">
+        <v>341</v>
+      </c>
+      <c r="C347" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="348" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>201</v>
+      </c>
+      <c r="B348" t="s">
         <v>348</v>
       </c>
-      <c r="C345" t="s">
+      <c r="C348" t="s">
         <v>300</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C345">
-    <sortCondition ref="A1:A345"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C348">
+    <sortCondition ref="A1:A348"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>